<commit_message>
Plotting on a canvas is done. Remaining points: making it interactive with an API and serving the index.html
</commit_message>
<xml_diff>
--- a/points.xlsx
+++ b/points.xlsx
@@ -345,706 +345,1410 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>5.005649060618551</v>
+        <v>5.0094546978990016</v>
       </c>
       <c r="B2">
         <v>0.01</v>
       </c>
       <c r="C2">
-        <v>2.4000666898938077</v>
+        <v>1.2001753806584528</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>5.288074533715215</v>
+        <v>5.482068439914272</v>
       </c>
       <c r="B3">
         <v>0.51</v>
       </c>
       <c r="C3">
-        <v>2.3999946404083485</v>
+        <v>1.2003889829027083</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>5.5700822812602295</v>
+        <v>5.953717911377767</v>
       </c>
       <c r="B4">
         <v>1.01</v>
       </c>
       <c r="C4">
-        <v>2.399925362904066</v>
+        <v>1.2007466692484685</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>5.85062741741292</v>
+        <v>6.4231768843825625</v>
       </c>
       <c r="B5">
         <v>1.51</v>
       </c>
       <c r="C5">
-        <v>2.400291348426053</v>
+        <v>1.2007558572919899</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>6.128922871084468</v>
+        <v>6.889539824003493</v>
       </c>
       <c r="B6">
         <v>2.0100000000000002</v>
       </c>
       <c r="C6">
-        <v>2.3999523977471777</v>
+        <v>1.199844867316632</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6.4033428066816285</v>
+        <v>7.3489570027540445</v>
       </c>
       <c r="B7">
         <v>2.5100000000000002</v>
       </c>
       <c r="C7">
-        <v>2.4000256090247922</v>
+        <v>1.2005166535502578</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>6.672529784916268</v>
+        <v>7.803631034151827</v>
       </c>
       <c r="B8">
         <v>3.0100000000000002</v>
       </c>
       <c r="C8">
-        <v>2.400578014490392</v>
+        <v>1.1994667090869904</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>6.937244378012249</v>
+        <v>8.247569942057915</v>
       </c>
       <c r="B9">
         <v>3.5100000000000002</v>
       </c>
       <c r="C9">
-        <v>2.399117941394176</v>
+        <v>1.2005027260129209</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>7.193801019341357</v>
+        <v>8.684013684075564</v>
       </c>
       <c r="B10">
         <v>4.010000000000001</v>
       </c>
       <c r="C10">
-        <v>2.399481788956844</v>
+        <v>1.2006896677062864</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>7.441852842899561</v>
+        <v>9.111427929786652</v>
       </c>
       <c r="B11">
         <v>4.510000000000001</v>
       </c>
       <c r="C11">
-        <v>2.400682721344296</v>
+        <v>1.2007998566631768</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>7.684679933312535</v>
+        <v>9.531098478962305</v>
       </c>
       <c r="B12">
         <v>5.010000000000001</v>
       </c>
       <c r="C12">
-        <v>2.39901295415096</v>
+        <v>1.200138219092883</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>7.916937753793271</v>
+        <v>9.941021459617183</v>
       </c>
       <c r="B13">
         <v>5.510000000000001</v>
       </c>
       <c r="C13">
-        <v>2.3992041975053096</v>
+        <v>1.1996423007268988</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>8.139762397127235</v>
+        <v>10.341503628797044</v>
       </c>
       <c r="B14">
         <v>6.010000000000001</v>
       </c>
       <c r="C14">
-        <v>2.399679016901615</v>
+        <v>1.1991289413477084</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>8.354192966412068</v>
+        <v>10.731007882942711</v>
       </c>
       <c r="B15">
         <v>6.510000000000001</v>
       </c>
       <c r="C15">
-        <v>2.399464956962287</v>
+        <v>1.1991371414582155</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>8.558391424531365</v>
+        <v>11.110116050230731</v>
       </c>
       <c r="B16">
         <v>7.010000000000001</v>
       </c>
       <c r="C16">
-        <v>2.3997529690355504</v>
+        <v>1.1993944218099335</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>8.753067086553626</v>
+        <v>11.47940837805946</v>
       </c>
       <c r="B17">
         <v>7.510000000000001</v>
       </c>
       <c r="C17">
-        <v>2.399927489748282</v>
+        <v>1.199710477435468</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>8.937840039020365</v>
+        <v>11.842176166474133</v>
       </c>
       <c r="B18">
         <v>8.010000000000002</v>
       </c>
       <c r="C18">
-        <v>2.4001603317637135</v>
+        <v>1.199171313491785</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>9.113456987985646</v>
+        <v>12.188667584828208</v>
       </c>
       <c r="B19">
         <v>8.510000000000002</v>
       </c>
       <c r="C19">
-        <v>2.4000061711027048</v>
+        <v>1.2005999700736365</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>9.276942202427481</v>
+        <v>12.52962020435073</v>
       </c>
       <c r="B20">
         <v>9.010000000000002</v>
       </c>
       <c r="C20">
-        <v>2.400978872862118</v>
+        <v>1.2009761930869176</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>9.433092915337944</v>
+        <v>12.868191585719064</v>
       </c>
       <c r="B21">
         <v>9.510000000000002</v>
       </c>
       <c r="C21">
-        <v>2.400625888891661</v>
+        <v>1.1997268879217171</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>9.579026394236644</v>
+        <v>13.190503270725452</v>
       </c>
       <c r="B22">
         <v>10.010000000000002</v>
       </c>
       <c r="C22">
-        <v>2.4004214462252</v>
+        <v>1.2003502684461091</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>9.713356360417208</v>
+        <v>13.509512210097082</v>
       </c>
       <c r="B23">
         <v>10.510000000000002</v>
       </c>
       <c r="C23">
-        <v>2.4009165564510937</v>
+        <v>1.1997547941804632</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>9.841227785544785</v>
+        <v>13.813112458711613</v>
       </c>
       <c r="B24">
         <v>11.010000000000002</v>
       </c>
       <c r="C24">
-        <v>2.3999408529121835</v>
+        <v>1.2007068904547396</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>9.954978961718417</v>
+        <v>14.118832508417153</v>
       </c>
       <c r="B25">
         <v>11.510000000000002</v>
       </c>
       <c r="C25">
-        <v>2.400612412522796</v>
+        <v>1.1994782168928524</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>10.061572559007248</v>
+        <v>14.408216774419392</v>
       </c>
       <c r="B26">
         <v>12.010000000000002</v>
       </c>
       <c r="C26">
-        <v>2.4001664859018788</v>
+        <v>1.1999700623213594</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>10.159180714441002</v>
+        <v>14.68762120807213</v>
       </c>
       <c r="B27">
         <v>12.510000000000002</v>
       </c>
       <c r="C27">
-        <v>2.3993756018331815</v>
+        <v>1.2008191260775274</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>10.244721016056596</v>
+        <v>14.963613718865892</v>
       </c>
       <c r="B28">
         <v>13.010000000000002</v>
       </c>
       <c r="C28">
-        <v>2.3992916216542013</v>
+        <v>1.200823211374672</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>10.318891853815398</v>
+        <v>15.232044194905752</v>
       </c>
       <c r="B29">
         <v>13.510000000000002</v>
       </c>
       <c r="C29">
-        <v>2.399586257467595</v>
+        <v>1.2008227390836155</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>10.381474191557642</v>
+        <v>15.501307439620625</v>
       </c>
       <c r="B30">
         <v>14.010000000000002</v>
       </c>
       <c r="C30">
-        <v>2.4002571339604417</v>
+        <v>1.1994278620366172</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>10.439178290319784</v>
+        <v>15.748966008152458</v>
       </c>
       <c r="B31">
         <v>14.510000000000002</v>
       </c>
       <c r="C31">
-        <v>2.399293080950484</v>
+        <v>1.2004514650192313</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>10.4821857394373</v>
+        <v>15.992608408291433</v>
       </c>
       <c r="B32">
         <v>15.010000000000002</v>
       </c>
       <c r="C32">
-        <v>2.399590722561364</v>
+        <v>1.200908361621799</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>10.511333808815525</v>
+        <v>16.23444602774411</v>
       </c>
       <c r="B33">
         <v>15.510000000000002</v>
       </c>
       <c r="C33">
-        <v>2.4007443386937264</v>
+        <v>1.2005333438390922</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>10.535256749823741</v>
+        <v>16.471728900363505</v>
       </c>
       <c r="B34">
         <v>16.01</v>
       </c>
       <c r="C34">
-        <v>2.4004192905369726</v>
+        <v>1.1998269564784265</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>10.546782995232578</v>
+        <v>16.698512941108426</v>
       </c>
       <c r="B35">
         <v>16.51</v>
       </c>
       <c r="C35">
-        <v>2.4005051113217375</v>
+        <v>1.1996845751305945</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>10.546782995232578</v>
+        <v>16.91417671198939</v>
       </c>
       <c r="B36">
         <v>17.01</v>
       </c>
       <c r="C36">
-        <v>2.4007094011699435</v>
+        <v>1.2001558992235335</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>10.53628029773141</v>
+        <v>17.122521685526696</v>
       </c>
       <c r="B37">
         <v>17.51</v>
       </c>
       <c r="C37">
-        <v>2.400744224748664</v>
+        <v>1.200688545587081</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>10.516023602542784</v>
+        <v>17.33065560909747</v>
       </c>
       <c r="B38">
         <v>18.01</v>
       </c>
       <c r="C38">
-        <v>2.400420884576064</v>
+        <v>1.2003590548122107</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>10.486975252751545</v>
+        <v>17.53971420980387</v>
       </c>
       <c r="B39">
         <v>18.51</v>
       </c>
       <c r="C39">
-        <v>2.3995332054549787</v>
+        <v>1.1991068805093517</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>10.43790093316924</v>
+        <v>17.72162778114703</v>
       </c>
       <c r="B40">
         <v>19.01</v>
       </c>
       <c r="C40">
-        <v>2.4003143236312696</v>
+        <v>1.2004849824742572</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>10.380315473149587</v>
+        <v>17.906874370478057</v>
       </c>
       <c r="B41">
         <v>19.51</v>
       </c>
       <c r="C41">
-        <v>2.4003209139221027</v>
+        <v>1.2006272592417118</v>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>10.311876819809282</v>
+        <v>18.088041419679552</v>
       </c>
       <c r="B42">
         <v>20.01</v>
       </c>
       <c r="C42">
-        <v>2.4000033982601314</v>
+        <v>1.2005063048629707</v>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>10.226659340612722</v>
+        <v>18.260265850116888</v>
       </c>
       <c r="B43">
         <v>20.51</v>
       </c>
       <c r="C43">
-        <v>2.4003591468913554</v>
+        <v>1.200704349497694</v>
       </c>
     </row>
     <row r="44">
       <c r="A44">
-        <v>10.131170969091338</v>
+        <v>18.440261161803818</v>
       </c>
       <c r="B44">
         <v>21.01</v>
       </c>
       <c r="C44">
-        <v>2.400143280875691</v>
+        <v>1.1993483916480199</v>
       </c>
     </row>
     <row r="45">
       <c r="A45">
-        <v>10.019692842321948</v>
+        <v>18.587834574280162</v>
       </c>
       <c r="B45">
         <v>21.51</v>
       </c>
       <c r="C45">
-        <v>2.4002507494198544</v>
+        <v>1.2009105607643307</v>
       </c>
     </row>
     <row r="46">
       <c r="A46">
-        <v>9.890389806866878</v>
+        <v>18.7443441413956</v>
       </c>
       <c r="B46">
         <v>22.01</v>
       </c>
       <c r="C46">
-        <v>2.4008248937647516</v>
+        <v>1.2008164339923058</v>
       </c>
     </row>
     <row r="47">
       <c r="A47">
-        <v>9.754541562159824</v>
+        <v>18.895949491533965</v>
       </c>
       <c r="B47">
         <v>22.51</v>
       </c>
       <c r="C47">
-        <v>2.4000631915779023</v>
+        <v>1.2006160956474323</v>
       </c>
     </row>
     <row r="48">
       <c r="A48">
-        <v>9.593984430581942</v>
+        <v>19.055053386252684</v>
       </c>
       <c r="B48">
         <v>23.01</v>
       </c>
       <c r="C48">
-        <v>2.400543864613358</v>
+        <v>1.1990774434147742</v>
       </c>
     </row>
     <row r="49">
       <c r="A49">
-        <v>9.41792855799209</v>
+        <v>19.176862266382404</v>
       </c>
       <c r="B49">
         <v>23.51</v>
       </c>
       <c r="C49">
-        <v>2.4007593471064896</v>
+        <v>1.2006880134971067</v>
       </c>
     </row>
     <row r="50">
       <c r="A50">
-        <v>9.229569986832248</v>
+        <v>19.307536773372238</v>
       </c>
       <c r="B50">
         <v>24.01</v>
       </c>
       <c r="C50">
-        <v>2.4002051835225893</v>
+        <v>1.2008148812266237</v>
       </c>
     </row>
     <row r="51">
       <c r="A51">
-        <v>9.01094440075012</v>
+        <v>19.434208224636933</v>
       </c>
       <c r="B51">
         <v>24.51</v>
       </c>
       <c r="C51">
-        <v>2.4009728684737137</v>
+        <v>1.200765688362567</v>
       </c>
     </row>
     <row r="52">
       <c r="A52">
-        <v>8.78200677184899</v>
+        <v>19.5617107325379</v>
       </c>
       <c r="B52">
         <v>25.01</v>
       </c>
       <c r="C52">
-        <v>2.4004435626161964</v>
+        <v>1.2001143637851759</v>
       </c>
     </row>
     <row r="53">
       <c r="A53">
-        <v>8.536655066657072</v>
+        <v>19.67044200395837</v>
       </c>
       <c r="B53">
         <v>25.51</v>
       </c>
       <c r="C53">
-        <v>2.399271628467998</v>
+        <v>1.200652189341238</v>
       </c>
     </row>
     <row r="54">
       <c r="A54">
-        <v>8.251012862999538</v>
+        <v>19.784758152719238</v>
       </c>
       <c r="B54">
         <v>26.01</v>
       </c>
       <c r="C54">
-        <v>2.39973298663006</v>
+        <v>1.2001789787364392</v>
       </c>
     </row>
     <row r="55">
       <c r="A55">
-        <v>7.932928087171678</v>
+        <v>19.882996101411727</v>
       </c>
       <c r="B55">
         <v>26.51</v>
       </c>
       <c r="C55">
-        <v>2.4005471072812674</v>
+        <v>1.2006088870602782</v>
       </c>
     </row>
     <row r="56">
       <c r="A56">
-        <v>7.608567198963323</v>
+        <v>19.981721834412163</v>
       </c>
       <c r="B56">
         <v>27.01</v>
       </c>
       <c r="C56">
-        <v>2.39904685224761</v>
+        <v>1.2005042241789805</v>
       </c>
     </row>
     <row r="57">
       <c r="A57">
-        <v>7.228682278292655</v>
+        <v>20.06909485214731</v>
       </c>
       <c r="B57">
         <v>27.51</v>
       </c>
       <c r="C57">
-        <v>2.3993113512838833</v>
+        <v>1.2008651498018454</v>
       </c>
     </row>
     <row r="58">
       <c r="A58">
-        <v>6.810420727977042</v>
+        <v>20.163667456617723</v>
       </c>
       <c r="B58">
         <v>28.01</v>
       </c>
       <c r="C58">
-        <v>2.399243346618662</v>
+        <v>1.2001848180500452</v>
       </c>
     </row>
     <row r="59">
       <c r="A59">
-        <v>6.327147227523432</v>
+        <v>20.234797266411867</v>
       </c>
       <c r="B59">
         <v>28.51</v>
       </c>
       <c r="C59">
-        <v>2.4001342421404757</v>
+        <v>1.2009180161577448</v>
       </c>
     </row>
     <row r="60">
       <c r="A60">
-        <v>5.78868787721486</v>
+        <v>20.313046037072496</v>
       </c>
       <c r="B60">
         <v>29.01</v>
       </c>
       <c r="C60">
-        <v>2.400345166241718</v>
+        <v>1.2006453318776733</v>
       </c>
     </row>
     <row r="61">
       <c r="A61">
-        <v>5.163651718771062</v>
+        <v>20.384702798128746</v>
       </c>
       <c r="B61">
         <v>29.51</v>
       </c>
       <c r="C61">
-        <v>2.400655110853279</v>
+        <v>1.2004533428342643</v>
       </c>
     </row>
     <row r="62">
       <c r="A62">
-        <v>4.4400336980370625</v>
+        <v>20.45146269979262</v>
       </c>
       <c r="B62">
         <v>30.01</v>
       </c>
       <c r="C62">
-        <v>2.399977829714982</v>
+        <v>1.200213339148072</v>
       </c>
     </row>
     <row r="63">
       <c r="A63">
-        <v>3.5311909458928494</v>
+        <v>20.518441240134447</v>
       </c>
       <c r="B63">
         <v>30.51</v>
       </c>
       <c r="C63">
-        <v>2.3992930053876935</v>
+        <v>1.1995631993365288</v>
       </c>
     </row>
     <row r="64">
       <c r="A64">
-        <v>2.1857276897713556</v>
+        <v>20.55301105979178</v>
       </c>
       <c r="B64">
         <v>31.01</v>
       </c>
       <c r="C64">
-        <v>2.399305581812894</v>
+        <v>1.2008079971114796</v>
       </c>
     </row>
     <row r="65">
       <c r="A65">
-        <v>0.001954840091327651</v>
+        <v>20.620322171012603</v>
       </c>
       <c r="B65">
         <v>31.51</v>
       </c>
       <c r="C65">
-        <v>2.3846519244469273</v>
+        <v>1.199372165637327</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66">
+        <v>20.637685595735416</v>
+      </c>
+      <c r="B66">
+        <v>32.010000000000005</v>
+      </c>
+      <c r="C66">
+        <v>1.2009585525542914</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67">
+        <v>20.67245632031628</v>
+      </c>
+      <c r="B67">
+        <v>32.510000000000005</v>
+      </c>
+      <c r="C67">
+        <v>1.2009625987875852</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68">
+        <v>20.702072886658076</v>
+      </c>
+      <c r="B68">
+        <v>33.010000000000005</v>
+      </c>
+      <c r="C68">
+        <v>1.2009282965961423</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69">
+        <v>20.724722279855563</v>
+      </c>
+      <c r="B69">
+        <v>33.510000000000005</v>
+      </c>
+      <c r="C69">
+        <v>1.2009704409697792</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70">
+        <v>20.74217361510742</v>
+      </c>
+      <c r="B70">
+        <v>34.010000000000005</v>
+      </c>
+      <c r="C70">
+        <v>1.200973641172603</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71">
+        <v>20.754413725458647</v>
+      </c>
+      <c r="B71">
+        <v>34.510000000000005</v>
+      </c>
+      <c r="C71">
+        <v>1.2009391236573723</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72">
+        <v>20.75963964532589</v>
+      </c>
+      <c r="B72">
+        <v>35.010000000000005</v>
+      </c>
+      <c r="C72">
+        <v>1.2009735250462514</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73">
+        <v>20.75963964532589</v>
+      </c>
+      <c r="B73">
+        <v>35.510000000000005</v>
+      </c>
+      <c r="C73">
+        <v>1.2009669252839936</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74">
+        <v>20.75963964532589</v>
+      </c>
+      <c r="B74">
+        <v>36.010000000000005</v>
+      </c>
+      <c r="C74">
+        <v>1.2006235658219553</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75">
+        <v>20.75963964532589</v>
+      </c>
+      <c r="B75">
+        <v>36.510000000000005</v>
+      </c>
+      <c r="C75">
+        <v>1.199961862861417</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76">
+        <v>20.726735780487818</v>
+      </c>
+      <c r="B76">
+        <v>37.010000000000005</v>
+      </c>
+      <c r="C76">
+        <v>1.2007846719891742</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77">
+        <v>20.726735780487818</v>
+      </c>
+      <c r="B77">
+        <v>37.510000000000005</v>
+      </c>
+      <c r="C77">
+        <v>1.1995006049535495</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78">
+        <v>20.671268376924015</v>
+      </c>
+      <c r="B78">
+        <v>38.010000000000005</v>
+      </c>
+      <c r="C78">
+        <v>1.2008345996785819</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79">
+        <v>20.63152649735729</v>
+      </c>
+      <c r="B79">
+        <v>38.510000000000005</v>
+      </c>
+      <c r="C79">
+        <v>1.2009945944850036</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80">
+        <v>20.591861024180474</v>
+      </c>
+      <c r="B80">
+        <v>39.010000000000005</v>
+      </c>
+      <c r="C80">
+        <v>1.2008291361328844</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81">
+        <v>20.540150915238215</v>
+      </c>
+      <c r="B81">
+        <v>39.510000000000005</v>
+      </c>
+      <c r="C81">
+        <v>1.2009466237323754</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82">
+        <v>20.485182836707025</v>
+      </c>
+      <c r="B82">
+        <v>40.010000000000005</v>
+      </c>
+      <c r="C82">
+        <v>1.200905346944369</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83">
+        <v>20.428596737334423</v>
+      </c>
+      <c r="B83">
+        <v>40.510000000000005</v>
+      </c>
+      <c r="C83">
+        <v>1.200634266147812</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84">
+        <v>20.372166945409393</v>
+      </c>
+      <c r="B84">
+        <v>41.010000000000005</v>
+      </c>
+      <c r="C84">
+        <v>1.200062493862893</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85">
+        <v>20.31589302916479</v>
+      </c>
+      <c r="B85">
+        <v>41.510000000000005</v>
+      </c>
+      <c r="C85">
+        <v>1.1992052482351265</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86">
+        <v>20.203811102608377</v>
+      </c>
+      <c r="B86">
+        <v>42.010000000000005</v>
+      </c>
+      <c r="C86">
+        <v>1.2005303553188096</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87">
+        <v>20.148002234712457</v>
+      </c>
+      <c r="B87">
+        <v>42.510000000000005</v>
+      </c>
+      <c r="C87">
+        <v>1.1990854770655703</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88">
+        <v>20.03684655460095</v>
+      </c>
+      <c r="B88">
+        <v>43.010000000000005</v>
+      </c>
+      <c r="C88">
+        <v>1.199726703776182</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89">
+        <v>19.92630411569704</v>
+      </c>
+      <c r="B89">
+        <v>43.510000000000005</v>
+      </c>
+      <c r="C89">
+        <v>1.2000176294781508</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90">
+        <v>19.816371534774788</v>
+      </c>
+      <c r="B90">
+        <v>44.010000000000005</v>
+      </c>
+      <c r="C90">
+        <v>1.1999745548493226</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91">
+        <v>19.7070454472734</v>
+      </c>
+      <c r="B91">
+        <v>44.510000000000005</v>
+      </c>
+      <c r="C91">
+        <v>1.1996133106309868</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92">
+        <v>19.549107363854688</v>
+      </c>
+      <c r="B92">
+        <v>45.010000000000005</v>
+      </c>
+      <c r="C92">
+        <v>1.2008349715467164</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93">
+        <v>19.442935573310066</v>
+      </c>
+      <c r="B93">
+        <v>45.510000000000005</v>
+      </c>
+      <c r="C93">
+        <v>1.199766812934665</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94">
+        <v>19.28225891020683</v>
+      </c>
+      <c r="B94">
+        <v>46.010000000000005</v>
+      </c>
+      <c r="C94">
+        <v>1.2004440396806302</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95">
+        <v>19.12291008105998</v>
+      </c>
+      <c r="B95">
+        <v>46.510000000000005</v>
+      </c>
+      <c r="C95">
+        <v>1.2007449922657945</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96">
+        <v>18.964878112633063</v>
+      </c>
+      <c r="B96">
+        <v>47.010000000000005</v>
+      </c>
+      <c r="C96">
+        <v>1.2006873036044787</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97">
+        <v>18.808152122372586</v>
+      </c>
+      <c r="B97">
+        <v>47.510000000000005</v>
+      </c>
+      <c r="C97">
+        <v>1.200288148484919</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98">
+        <v>18.652721317658656</v>
+      </c>
+      <c r="B98">
+        <v>48.010000000000005</v>
+      </c>
+      <c r="C98">
+        <v>1.1995642267035875</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99">
+        <v>18.447476490778545</v>
+      </c>
+      <c r="B99">
+        <v>48.510000000000005</v>
+      </c>
+      <c r="C99">
+        <v>1.2001841847034687</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100">
+        <v>18.24449007103611</v>
+      </c>
+      <c r="B100">
+        <v>49.010000000000005</v>
+      </c>
+      <c r="C100">
+        <v>1.2003967847992563</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101">
+        <v>18.043737208095905</v>
+      </c>
+      <c r="B101">
+        <v>49.510000000000005</v>
+      </c>
+      <c r="C101">
+        <v>1.2002220018525365</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102">
+        <v>17.84519332506261</v>
+      </c>
+      <c r="B102">
+        <v>50.010000000000005</v>
+      </c>
+      <c r="C102">
+        <v>1.199679297134521</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103">
+        <v>17.600082845394297</v>
+      </c>
+      <c r="B103">
+        <v>50.510000000000005</v>
+      </c>
+      <c r="C103">
+        <v>1.2002044021116578</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104">
+        <v>17.35833905086908</v>
+      </c>
+      <c r="B104">
+        <v>51.010000000000005</v>
+      </c>
+      <c r="C104">
+        <v>1.2002871601394012</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105">
+        <v>17.11991569879318</v>
+      </c>
+      <c r="B105">
+        <v>51.510000000000005</v>
+      </c>
+      <c r="C105">
+        <v>1.19995074764039</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106">
+        <v>16.88476718163372</v>
+      </c>
+      <c r="B106">
+        <v>52.010000000000005</v>
+      </c>
+      <c r="C106">
+        <v>1.199217706681459</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107">
+        <v>16.547071838001045</v>
+      </c>
+      <c r="B107">
+        <v>52.510000000000005</v>
+      </c>
+      <c r="C107">
+        <v>1.2008430060096154</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108">
+        <v>16.323900838800817</v>
+      </c>
+      <c r="B108">
+        <v>53.010000000000005</v>
+      </c>
+      <c r="C108">
+        <v>1.1991620767900868</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109">
+        <v>15.9974228220248</v>
+      </c>
+      <c r="B109">
+        <v>53.510000000000005</v>
+      </c>
+      <c r="C109">
+        <v>1.1997405937048422</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110">
+        <v>15.681421922274613</v>
+      </c>
+      <c r="B110">
+        <v>54.010000000000005</v>
+      </c>
+      <c r="C110">
+        <v>1.199679211235017</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111">
+        <v>15.371663063492763</v>
+      </c>
+      <c r="B111">
+        <v>54.510000000000005</v>
+      </c>
+      <c r="C111">
+        <v>1.1991137826088554</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112">
+        <v>14.942209540824901</v>
+      </c>
+      <c r="B112">
+        <v>55.010000000000005</v>
+      </c>
+      <c r="C112">
+        <v>1.2008183587402965</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113">
+        <v>14.643365350008404</v>
+      </c>
+      <c r="B113">
+        <v>55.510000000000005</v>
+      </c>
+      <c r="C113">
+        <v>1.19926906937099</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114">
+        <v>14.234259008859873</v>
+      </c>
+      <c r="B114">
+        <v>56.010000000000005</v>
+      </c>
+      <c r="C114">
+        <v>1.1996528564846167</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115">
+        <v>13.836582280670346</v>
+      </c>
+      <c r="B115">
+        <v>56.510000000000005</v>
+      </c>
+      <c r="C115">
+        <v>1.199363611266739</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116">
+        <v>13.410645103664704</v>
+      </c>
+      <c r="B116">
+        <v>57.010000000000005</v>
+      </c>
+      <c r="C116">
+        <v>1.1991800654879503</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117">
+        <v>12.882826610940208</v>
+      </c>
+      <c r="B117">
+        <v>57.510000000000005</v>
+      </c>
+      <c r="C117">
+        <v>1.200342139541431</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118">
+        <v>12.453817854778347</v>
+      </c>
+      <c r="B118">
+        <v>58.010000000000005</v>
+      </c>
+      <c r="C118">
+        <v>1.1992518071052465</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119">
+        <v>11.86376542972052</v>
+      </c>
+      <c r="B119">
+        <v>58.510000000000005</v>
+      </c>
+      <c r="C119">
+        <v>1.2002948144325631</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120">
+        <v>11.301669240122088</v>
+      </c>
+      <c r="B120">
+        <v>59.010000000000005</v>
+      </c>
+      <c r="C120">
+        <v>1.2002439662921813</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121">
+        <v>10.766204740793727</v>
+      </c>
+      <c r="B121">
+        <v>59.510000000000005</v>
+      </c>
+      <c r="C121">
+        <v>1.1992189657489825</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122">
+        <v>10.050987939640711</v>
+      </c>
+      <c r="B122">
+        <v>60.010000000000005</v>
+      </c>
+      <c r="C122">
+        <v>1.1999856816959136</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123">
+        <v>9.307279572602381</v>
+      </c>
+      <c r="B123">
+        <v>60.510000000000005</v>
+      </c>
+      <c r="C123">
+        <v>1.2002307035620152</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124">
+        <v>8.618600834345257</v>
+      </c>
+      <c r="B124">
+        <v>61.010000000000005</v>
+      </c>
+      <c r="C124">
+        <v>1.1990006408608487</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125">
+        <v>7.532346859587719</v>
+      </c>
+      <c r="B125">
+        <v>61.510000000000005</v>
+      </c>
+      <c r="C125">
+        <v>1.2008105128885145</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126">
+        <v>6.662936419252347</v>
+      </c>
+      <c r="B126">
+        <v>62.010000000000005</v>
+      </c>
+      <c r="C126">
+        <v>1.1992253354206548</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127">
+        <v>5.407226095807211</v>
+      </c>
+      <c r="B127">
+        <v>62.510000000000005</v>
+      </c>
+      <c r="C127">
+        <v>1.1991839101352082</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128">
+        <v>3.7080031863816183</v>
+      </c>
+      <c r="B128">
+        <v>63.010000000000005</v>
+      </c>
+      <c r="C128">
+        <v>1.1991566671549039</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129">
+        <v>0.0019608821103770705</v>
+      </c>
+      <c r="B129">
+        <v>63.510000000000005</v>
+      </c>
+      <c r="C129">
+        <v>1.197928805354223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>